<commit_message>
Fix for data type in TOC lookup
also 207 dimt table added to the solution for 207
</commit_message>
<xml_diff>
--- a/DataValidation/data validation for 105_TMILEAGE.xlsx
+++ b/DataValidation/data validation for 105_TMILEAGE.xlsx
@@ -200,7 +200,7 @@
     <t>No data shows as being outside 95% confidence interval for Year on Year change</t>
   </si>
   <si>
-    <t>Latest Load is source item id 9140</t>
+    <t>Latest Load is source item id 9202</t>
   </si>
   <si>
     <t>count</t>
@@ -227,7 +227,7 @@
     <t>max</t>
   </si>
   <si>
-    <t>Previous Load is source item id: 9126</t>
+    <t>Previous Load is source item id: 9140</t>
   </si>
 </sst>
 </file>

</xml_diff>